<commit_message>
Kommunikation weiter, Cardselector implementiert
</commit_message>
<xml_diff>
--- a/Bericht/Zeitplan.xlsx
+++ b/Bericht/Zeitplan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nick\Dokumente\GitHub\Tichu-Maturaarbeit\Bericht\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11160" windowHeight="4170"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Woche</t>
   </si>
@@ -27,9 +32,6 @@
     <t>Klassendiagramm</t>
   </si>
   <si>
-    <t>Programmieren</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -43,13 +45,31 @@
   </si>
   <si>
     <t>Ferien</t>
+  </si>
+  <si>
+    <t>Kommunikation</t>
+  </si>
+  <si>
+    <t>Spiellogik</t>
+  </si>
+  <si>
+    <t>Grafik</t>
+  </si>
+  <si>
+    <t>Programmieren:</t>
+  </si>
+  <si>
+    <t>Abgabe</t>
+  </si>
+  <si>
+    <t>(AndroidApp)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +109,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -102,13 +140,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -415,27 +459,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:AN15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="40" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.86328125" customWidth="1"/>
+    <col min="2" max="40" width="3.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -557,9 +601,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="14.25" customHeight="1">
+    <row r="5" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -574,9 +618,9 @@
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -587,7 +631,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -596,86 +640,183 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:40">
-      <c r="A10" t="s">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:40" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="1:40" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" s="4"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-    </row>
-    <row r="11" spans="1:40">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-    </row>
-    <row r="14" spans="1:40">
-      <c r="A14" t="s">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="4"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="4"/>
-    </row>
-    <row r="15" spans="1:40">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="4"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="4"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG27" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>